<commit_message>
Updated code to use ECI frame for thrust vector
- Refactored plotting code into functions for easier readability
- Added option to use ECI or RIC frame for thrust vector from STK
- Added functionality to save output plots into folder "Plot Comparisons"
</commit_message>
<xml_diff>
--- a/data_STK_astrogator/Processed_data/original/Lumelite2_final_summary.xlsx
+++ b/data_STK_astrogator/Processed_data/original/Lumelite2_final_summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ngengton\Documents\GitHub\FORMFLYT\data_STK_astrogator\Processed_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ngengton\Documents\GitHub\FORMFLYT\data_STK_astrogator\Processed_data\original\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FB0B04-10D8-44CB-B6EB-6F7107CA3225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2176519E-77B0-4233-8D02-FB52990A41B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1460" yWindow="1460" windowWidth="17280" windowHeight="8960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Segment Name</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>Delta V (m/sec)</t>
+  </si>
+  <si>
+    <t>ECI X Thrust Component</t>
+  </si>
+  <si>
+    <t>ECI Y Thrust Component</t>
+  </si>
+  <si>
+    <t>ECI Z Thrust Component</t>
   </si>
 </sst>
 </file>
@@ -463,15 +472,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -502,8 +511,17 @@
       <c r="K1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -523,7 +541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -543,7 +561,7 @@
         <v>43200</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -577,8 +595,17 @@
       <c r="K4">
         <v>-0.69539600000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>-0.65610000000000002</v>
+      </c>
+      <c r="M4">
+        <v>0.50031999999999999</v>
+      </c>
+      <c r="N4">
+        <v>-0.56494999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -598,7 +625,7 @@
         <v>1209600</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -632,8 +659,17 @@
       <c r="K6">
         <v>9.8040000000000002E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L6">
+        <v>-0.73919999999999997</v>
+      </c>
+      <c r="M6">
+        <v>0.66354000000000002</v>
+      </c>
+      <c r="N6">
+        <v>0.11472</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -653,7 +689,7 @@
         <v>28676</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -673,7 +709,7 @@
         <v>2101.4009999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -707,8 +743,17 @@
       <c r="K9">
         <v>-1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L9">
+        <v>0.10832</v>
+      </c>
+      <c r="M9">
+        <v>0.13139999999999999</v>
+      </c>
+      <c r="N9">
+        <v>-0.98538700000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -728,7 +773,7 @@
         <v>28676</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -748,7 +793,7 @@
         <v>5568.51</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -782,8 +827,17 @@
       <c r="K12">
         <v>-1</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L12">
+        <v>0.11428000000000001</v>
+      </c>
+      <c r="M12">
+        <v>0.12570999999999999</v>
+      </c>
+      <c r="N12">
+        <v>-0.98546</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -803,7 +857,7 @@
         <v>28676</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -823,7 +877,7 @@
         <v>5479.3980000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -857,8 +911,17 @@
       <c r="K15">
         <v>-1</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L15">
+        <v>0.11940000000000001</v>
+      </c>
+      <c r="M15">
+        <v>0.11965000000000001</v>
+      </c>
+      <c r="N15">
+        <v>-0.98560000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -878,7 +941,7 @@
         <v>28676</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -898,7 +961,7 @@
         <v>5491.973</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -932,8 +995,17 @@
       <c r="K18">
         <v>-1</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L18">
+        <v>0.12439</v>
+      </c>
+      <c r="M18">
+        <v>0.11327</v>
+      </c>
+      <c r="N18">
+        <v>-0.98570000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -953,7 +1025,7 @@
         <v>28676</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -973,7 +1045,7 @@
         <v>5575.2820000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1007,8 +1079,17 @@
       <c r="K21">
         <v>-1</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L21">
+        <v>0.12944</v>
+      </c>
+      <c r="M21">
+        <v>0.10666</v>
+      </c>
+      <c r="N21">
+        <v>-0.98582999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1028,7 +1109,7 @@
         <v>28676</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1048,7 +1129,7 @@
         <v>5518.366</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1082,8 +1163,17 @@
       <c r="K24">
         <v>-1</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L24">
+        <v>0.1338</v>
+      </c>
+      <c r="M24">
+        <v>9.9720000000000003E-2</v>
+      </c>
+      <c r="N24">
+        <v>-0.98597000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1103,7 +1193,7 @@
         <v>28676</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1123,7 +1213,7 @@
         <v>5547.7169999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1157,8 +1247,17 @@
       <c r="K27">
         <v>-1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L27">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="M27">
+        <v>9.2555999999999999E-2</v>
+      </c>
+      <c r="N27">
+        <v>-0.98609000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1178,7 +1277,7 @@
         <v>28676</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1198,7 +1297,7 @@
         <v>5528.81</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1232,8 +1331,17 @@
       <c r="K30">
         <v>-1</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L30">
+        <v>0.14172999999999999</v>
+      </c>
+      <c r="M30">
+        <v>8.5123000000000004E-2</v>
+      </c>
+      <c r="N30">
+        <v>-0.98623700000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>

</xml_diff>